<commit_message>
add Donut line chart
</commit_message>
<xml_diff>
--- a/input/ablition.xlsx
+++ b/input/ablition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Library/Mobile Documents/com~apple~CloudDocs/Research/CVPR2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7047887D-8785-944F-A82B-E1BA42096103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38279719-0786-524A-9AEB-AF9759ECFB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{32123199-82DE-4F44-98B8-550E7ABB68F9}"/>
   </bookViews>
@@ -77,22 +77,22 @@
     <t>lamda1-lamda2</t>
   </si>
   <si>
-    <t>1.0--1.0</t>
-  </si>
-  <si>
-    <t>1.0--0.1</t>
-  </si>
-  <si>
-    <t>0.9--0.1</t>
-  </si>
-  <si>
-    <t>0.8--0.2</t>
-  </si>
-  <si>
-    <t>0.7--0.3</t>
-  </si>
-  <si>
-    <t>0.6--0.4</t>
+    <t>1.0, 1.0</t>
+  </si>
+  <si>
+    <t>1.0, 0.1</t>
+  </si>
+  <si>
+    <t>0.9, 0.1</t>
+  </si>
+  <si>
+    <t>0.8, 0.2</t>
+  </si>
+  <si>
+    <t>0.7, 0.3</t>
+  </si>
+  <si>
+    <t>0.6, 0.4</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>